<commit_message>
added table info queries
</commit_message>
<xml_diff>
--- a/AssessmentList.xlsx
+++ b/AssessmentList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/nicksalc_microsoft_com1/Documents/Github/SynapseHealthAssessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="8_{333580E6-5367-4011-81E7-E0FF622FDD49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{60AA7543-19A2-47F4-8703-F6035C84ECAA}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="8_{333580E6-5367-4011-81E7-E0FF622FDD49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F107D62D-2953-4B5F-8C51-96025CDCFE33}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5C4F97EF-D37C-4010-B2B3-1260A2189393}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="173">
   <si>
     <t>Item</t>
   </si>
@@ -518,13 +518,52 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Link to query</t>
+  </si>
+  <si>
+    <t>https://github.com/microsoft/SynapseHealthAssessment/blob/main/SQL_Scripts/CciHealthByTable.sql</t>
+  </si>
+  <si>
+    <t>DBCC PDW_SHOWSPACEUSED</t>
+  </si>
+  <si>
+    <t>database size per distribution</t>
+  </si>
+  <si>
+    <t>SELECT * FROM sys.databases where name != 'master'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run against master, if &gt;2 then there are multiple user databases: SELECT COUNT(*) FROM sys.databases </t>
+  </si>
+  <si>
+    <t>Pre-Req view</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/microsoft/Azure_Synapse_Toolbox/master/SQL_Queries/Table_Information/CreateTableInfoView.sql</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/microsoft/Azure_Synapse_Toolbox/master/SQL_Queries/Indexes/CreateRowgroupHealthView.sql</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/microsoft/Azure_Synapse_Toolbox/master/SQL_Queries/Table_Information/TableSkew.sql</t>
+  </si>
+  <si>
+    <t>Fix link to point to healthassessment github</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Failed autostats jobs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +589,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -606,10 +653,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -620,8 +668,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -731,20 +781,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{798E3207-8B2C-47A9-883E-D74382C09352}" name="Table1" displayName="Table1" ref="A1:F63" totalsRowShown="0">
-  <autoFilter ref="A1:F63" xr:uid="{5703D66D-1822-4365-9273-C51F7109314D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F63">
-    <sortCondition ref="A2:A63"/>
-    <sortCondition ref="B2:B63"/>
-    <sortCondition ref="C2:C63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{798E3207-8B2C-47A9-883E-D74382C09352}" name="Table1" displayName="Table1" ref="A1:I65" totalsRowShown="0">
+  <autoFilter ref="A1:I65" xr:uid="{5703D66D-1822-4365-9273-C51F7109314D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G65">
+    <sortCondition ref="A1:A65"/>
   </sortState>
-  <tableColumns count="6">
+  <tableColumns count="9">
     <tableColumn id="12" xr3:uid="{AFD01177-99B2-4497-9E50-5BC575779994}" name="Category"/>
     <tableColumn id="1" xr3:uid="{8BACA63F-81DA-4522-B17C-D39F6BAFD188}" name="Sub-Category"/>
     <tableColumn id="2" xr3:uid="{2726D609-060B-4E14-9FA3-8D516E62ED14}" name="Test"/>
     <tableColumn id="3" xr3:uid="{59D8DB47-2BC5-4715-8454-8DD879E7250B}" name="Summary" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{7634C1FE-6EAD-4A81-9708-EF2CC045EB17}" name="Collected by "/>
     <tableColumn id="5" xr3:uid="{50BD6E41-76DB-4D3E-B5CA-D6A176F9A73E}" name="Status"/>
+    <tableColumn id="6" xr3:uid="{06E5D75F-7411-4EFA-902F-E7339CDED8A3}" name="Link to query"/>
+    <tableColumn id="7" xr3:uid="{974B7D4C-6CB3-4F7C-A8C9-DC06624CB7EE}" name="Pre-Req view"/>
+    <tableColumn id="8" xr3:uid="{DBEF767F-D1EE-4551-8F4C-6EE91253C096}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1092,7 +1143,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1214,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FB388A-8907-42F8-9F51-A2DBE026E81A}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1225,12 +1276,14 @@
     <col min="1" max="1" width="25.59765625" customWidth="1"/>
     <col min="2" max="2" width="25.1328125" customWidth="1"/>
     <col min="3" max="3" width="49" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92.86328125" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" customWidth="1"/>
     <col min="5" max="5" width="31.265625" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="88.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="118.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1249,8 +1302,17 @@
       <c r="F1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1261,8 +1323,11 @@
         <v>30</v>
       </c>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H2" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1274,7 +1339,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1291,7 +1356,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1303,7 +1368,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1318,7 +1383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1332,8 +1397,11 @@
       <c r="E7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G7" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1350,7 +1418,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1364,8 +1432,17 @@
       <c r="E9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="I9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1380,7 +1457,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1395,7 +1472,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1410,7 +1487,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1425,7 +1502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1433,11 +1510,14 @@
         <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>172</v>
       </c>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1445,11 +1525,11 @@
         <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1457,11 +1537,14 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1469,11 +1552,11 @@
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1481,16 +1564,11 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1498,207 +1576,224 @@
         <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>28</v>
       </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
       <c r="C20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="G28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>59</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>79</v>
-      </c>
-      <c r="B31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -1706,53 +1801,59 @@
         <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>79</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -1760,14 +1861,11 @@
         <v>92</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -1775,11 +1873,11 @@
         <v>92</v>
       </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1787,59 +1885,62 @@
         <v>92</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>79</v>
       </c>
+      <c r="B41" t="s">
+        <v>92</v>
+      </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>79</v>
       </c>
+      <c r="B42" t="s">
+        <v>92</v>
+      </c>
       <c r="C42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" t="s">
+      <c r="D44" s="1"/>
+      <c r="E44" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>102</v>
-      </c>
-      <c r="B43" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -1847,47 +1948,44 @@
         <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>102</v>
       </c>
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
       <c r="C46" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" t="s">
         <v>107</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" t="s">
-        <v>111</v>
-      </c>
-      <c r="D47" s="1"/>
-      <c r="E47" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>109</v>
-      </c>
-      <c r="B48" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" t="s">
-        <v>112</v>
-      </c>
-      <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
@@ -1897,11 +1995,11 @@
         <v>110</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
@@ -1912,7 +2010,7 @@
         <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D50" s="1"/>
     </row>
@@ -1924,9 +2022,12 @@
         <v>110</v>
       </c>
       <c r="C51" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D51" s="1"/>
+      <c r="E51" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
@@ -1936,12 +2037,9 @@
         <v>110</v>
       </c>
       <c r="C52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D52" s="1"/>
-      <c r="E52" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
@@ -1951,12 +2049,9 @@
         <v>110</v>
       </c>
       <c r="C53" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
@@ -1966,10 +2061,11 @@
         <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>119</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
@@ -1980,10 +2076,11 @@
         <v>110</v>
       </c>
       <c r="C55" t="s">
-        <v>121</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
@@ -1994,9 +2091,11 @@
         <v>110</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
-      </c>
-      <c r="D56" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
@@ -2006,10 +2105,10 @@
         <v>110</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
@@ -2017,10 +2116,10 @@
         <v>109</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="C58" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D58" s="1"/>
     </row>
@@ -2029,13 +2128,13 @@
         <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
@@ -2043,10 +2142,10 @@
         <v>109</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D60" s="1"/>
     </row>
@@ -2054,35 +2153,67 @@
       <c r="A61" t="s">
         <v>109</v>
       </c>
+      <c r="B61" t="s">
+        <v>127</v>
+      </c>
       <c r="C61" t="s">
-        <v>131</v>
-      </c>
-      <c r="D61" s="1"/>
-      <c r="E61" t="s">
-        <v>100</v>
+        <v>128</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>109</v>
       </c>
+      <c r="B62" t="s">
+        <v>103</v>
+      </c>
       <c r="C62" t="s">
+        <v>130</v>
+      </c>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>109</v>
+      </c>
+      <c r="C63" t="s">
+        <v>131</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" t="s">
         <v>132</v>
       </c>
-      <c r="D62" s="1"/>
-      <c r="E62" t="s">
+      <c r="D64" s="1"/>
+      <c r="E64" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D63" s="1"/>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D65" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{8B2E3FCF-FBAA-4D89-A2BD-D0D0F585DA43}"/>
+    <hyperlink ref="G7" r:id="rId2" xr:uid="{114B2659-B33C-4854-87B4-B4D768A329CE}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{9509FFA4-0C2B-4706-B902-30D3FD56DF94}"/>
+    <hyperlink ref="G9" r:id="rId4" xr:uid="{88FEA10A-7BB4-4841-90E3-AAA6EDA79E90}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2367,6 +2498,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046C9DBCDDFD8DB418F41B2241B54161A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7033472e0bb57c6599fdcbd9f7677219">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="58e001b3-03d5-4b34-abf9-59e2cfe2e3d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6444ba373961e4493ffb4522bc49aff9" ns2:_="">
     <xsd:import namespace="58e001b3-03d5-4b34-abf9-59e2cfe2e3d0"/>
@@ -2512,22 +2658,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9875775B-611E-456C-9690-799BC8577167}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024609E9-C262-4587-9050-8BFE45D722CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB5C63C8-7919-4159-800E-C7653F629984}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2545,23 +2693,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{024609E9-C262-4587-9050-8BFE45D722CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9875775B-611E-456C-9690-799BC8577167}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>